<commit_message>
Import descriptions from spreadsheets
</commit_message>
<xml_diff>
--- a/test/fixtures/spreadsheets/empty_valid_spreadsheet.xlsx
+++ b/test/fixtures/spreadsheets/empty_valid_spreadsheet.xlsx
@@ -29,7 +29,7 @@
     <t>Resource Subtitle</t>
   </si>
   <si>
-    <t>URL</t>
+    <t>Resource Description</t>
   </si>
 </sst>
 </file>
@@ -44,6 +44,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,10 +130,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -140,7 +141,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -157,7 +158,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>